<commit_message>
adding the subjects table
</commit_message>
<xml_diff>
--- a/departments.xlsx
+++ b/departments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claire Norman\Desktop\zagsabroad\zags-abroad-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF3E2D1-0534-4394-B749-3C8CC99A9284}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14812400-9C62-4D47-8922-DE1017B72120}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="6825" windowHeight="1208" xr2:uid="{9EE62BB4-A12E-47E8-B063-BD7085D631FB}"/>
   </bookViews>
@@ -677,7 +677,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="C28" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -694,9 +694,6 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
@@ -707,9 +704,6 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
@@ -718,9 +712,6 @@
       <c r="B3" t="s">
         <v>64</v>
       </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
@@ -729,9 +720,6 @@
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
@@ -740,9 +728,6 @@
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
@@ -751,9 +736,6 @@
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6">
-        <v>6</v>
-      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
@@ -762,9 +744,6 @@
       <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7">
-        <v>7</v>
-      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
@@ -773,9 +752,6 @@
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8">
-        <v>8</v>
-      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
@@ -784,9 +760,6 @@
       <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="C9">
-        <v>9</v>
-      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
@@ -795,9 +768,6 @@
       <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C10">
-        <v>10</v>
-      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
@@ -806,9 +776,6 @@
       <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C11">
-        <v>11</v>
-      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
@@ -817,9 +784,6 @@
       <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="C12">
-        <v>12</v>
-      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
@@ -828,9 +792,6 @@
       <c r="B13" t="s">
         <v>12</v>
       </c>
-      <c r="C13">
-        <v>13</v>
-      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
@@ -839,9 +800,6 @@
       <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="C14">
-        <v>14</v>
-      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
@@ -850,9 +808,6 @@
       <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="C15">
-        <v>15</v>
-      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
@@ -861,9 +816,6 @@
       <c r="B16" t="s">
         <v>15</v>
       </c>
-      <c r="C16">
-        <v>16</v>
-      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
@@ -872,9 +824,6 @@
       <c r="B17" t="s">
         <v>65</v>
       </c>
-      <c r="C17">
-        <v>17</v>
-      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
@@ -883,9 +832,6 @@
       <c r="B18" t="s">
         <v>66</v>
       </c>
-      <c r="C18">
-        <v>18</v>
-      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
@@ -894,9 +840,6 @@
       <c r="B19" t="s">
         <v>0</v>
       </c>
-      <c r="C19">
-        <v>19</v>
-      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
@@ -905,9 +848,6 @@
       <c r="B20" t="s">
         <v>67</v>
       </c>
-      <c r="C20">
-        <v>20</v>
-      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
@@ -916,9 +856,6 @@
       <c r="B21" t="s">
         <v>68</v>
       </c>
-      <c r="C21">
-        <v>21</v>
-      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
@@ -927,9 +864,6 @@
       <c r="B22" t="s">
         <v>69</v>
       </c>
-      <c r="C22">
-        <v>22</v>
-      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
@@ -938,9 +872,6 @@
       <c r="B23" t="s">
         <v>70</v>
       </c>
-      <c r="C23">
-        <v>23</v>
-      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
@@ -949,9 +880,6 @@
       <c r="B24" t="s">
         <v>71</v>
       </c>
-      <c r="C24">
-        <v>24</v>
-      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
@@ -960,9 +888,6 @@
       <c r="B25" t="s">
         <v>72</v>
       </c>
-      <c r="C25">
-        <v>25</v>
-      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
@@ -971,9 +896,6 @@
       <c r="B26" t="s">
         <v>73</v>
       </c>
-      <c r="C26">
-        <v>26</v>
-      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
@@ -982,9 +904,6 @@
       <c r="B27" t="s">
         <v>74</v>
       </c>
-      <c r="C27">
-        <v>27</v>
-      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
@@ -993,9 +912,6 @@
       <c r="B28" t="s">
         <v>43</v>
       </c>
-      <c r="C28">
-        <v>28</v>
-      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
@@ -1004,9 +920,6 @@
       <c r="B29" t="s">
         <v>75</v>
       </c>
-      <c r="C29">
-        <v>29</v>
-      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
@@ -1015,9 +928,6 @@
       <c r="B30" t="s">
         <v>76</v>
       </c>
-      <c r="C30">
-        <v>30</v>
-      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
@@ -1026,9 +936,6 @@
       <c r="B31" t="s">
         <v>77</v>
       </c>
-      <c r="C31">
-        <v>31</v>
-      </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
@@ -1039,195 +946,141 @@
       <c r="B32" t="s">
         <v>78</v>
       </c>
-      <c r="C32">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>47</v>
       </c>
       <c r="B33" t="s">
         <v>79</v>
       </c>
-      <c r="C33">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>48</v>
       </c>
       <c r="B34" t="s">
         <v>80</v>
       </c>
-      <c r="C34">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>49</v>
       </c>
       <c r="B35" t="s">
         <v>81</v>
       </c>
-      <c r="C35">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>50</v>
       </c>
       <c r="B36" t="s">
         <v>82</v>
       </c>
-      <c r="C36">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>51</v>
       </c>
       <c r="B37" t="s">
         <v>83</v>
       </c>
-      <c r="C37">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>52</v>
       </c>
       <c r="B38" t="s">
         <v>84</v>
       </c>
-      <c r="C38">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>53</v>
       </c>
       <c r="B39" t="s">
         <v>85</v>
       </c>
-      <c r="C39">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>54</v>
       </c>
       <c r="B40" t="s">
         <v>86</v>
       </c>
-      <c r="C40">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>55</v>
       </c>
       <c r="B41" t="s">
         <v>87</v>
       </c>
-      <c r="C41">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>56</v>
       </c>
       <c r="B42" t="s">
         <v>88</v>
       </c>
-      <c r="C42">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>57</v>
       </c>
       <c r="B43" t="s">
         <v>89</v>
       </c>
-      <c r="C43">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>58</v>
       </c>
       <c r="B44" t="s">
         <v>90</v>
       </c>
-      <c r="C44">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>59</v>
       </c>
       <c r="B45" t="s">
         <v>91</v>
       </c>
-      <c r="C45">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>60</v>
       </c>
       <c r="B46" t="s">
         <v>92</v>
       </c>
-      <c r="C46">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>61</v>
       </c>
       <c r="B47" t="s">
         <v>93</v>
       </c>
-      <c r="C47">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>62</v>
       </c>
       <c r="B48" t="s">
         <v>94</v>
       </c>
-      <c r="C48">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>63</v>
       </c>
       <c r="B49" t="s">
         <v>95</v>
-      </c>
-      <c r="C49">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>